<commit_message>
API Get and Post request code written
</commit_message>
<xml_diff>
--- a/resources/APITestCases.xlsx
+++ b/resources/APITestCases.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26623"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAB65A2B-9744-4F6B-A890-047C434FDA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C78878C-ED71-49C2-A720-D5B98C6F3A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -66,68 +66,74 @@
     <t>SqlQuery</t>
   </si>
   <si>
+    <t>List_Users</t>
+  </si>
+  <si>
+    <t>https://reqres.in/api/users?page=1</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>Accept</t>
+  </si>
+  <si>
+    <t>*/*</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>select * from abc;</t>
+  </si>
+  <si>
+    <t>Accept-Encoding</t>
+  </si>
+  <si>
+    <t>zip,deflate,br</t>
+  </si>
+  <si>
+    <t>Connection</t>
+  </si>
+  <si>
+    <t>keep-alive</t>
+  </si>
+  <si>
+    <t>Content-Type</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>Authorization</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Test02</t>
+  </si>
+  <si>
+    <t>abc.com</t>
+  </si>
+  <si>
     <t>JWT</t>
   </si>
   <si>
-    <t>abc.com</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
-    <t>Accept</t>
-  </si>
-  <si>
-    <t>*/*</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
-    <t>select * from abc;</t>
-  </si>
-  <si>
-    <t>Accept-Encoding</t>
-  </si>
-  <si>
-    <t>zip,deflate,br</t>
-  </si>
-  <si>
     <t>token</t>
   </si>
   <si>
-    <t>Connection</t>
-  </si>
-  <si>
-    <t>keep-alive</t>
-  </si>
-  <si>
     <t>error</t>
-  </si>
-  <si>
-    <t>Content-Type</t>
-  </si>
-  <si>
-    <t>application/json</t>
-  </si>
-  <si>
-    <t>Authorization</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>Test02</t>
-  </si>
-  <si>
-    <t>data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +158,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -280,10 +294,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -312,8 +327,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -626,16 +651,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
@@ -688,7 +713,7 @@
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -705,7 +730,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="6"/>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="6" t="s">
@@ -714,7 +739,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -727,73 +752,69 @@
         <v>20</v>
       </c>
       <c r="J3" s="7"/>
-      <c r="K3" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="J4" s="7"/>
-      <c r="K4" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J5" s="7"/>
-      <c r="K5" s="5"/>
+      <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J6" s="8"/>
-      <c r="K6" s="5"/>
+      <c r="K6" s="8"/>
       <c r="L6" s="8"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>14</v>
@@ -810,7 +831,7 @@
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="9" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>18</v>
@@ -843,10 +864,10 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
@@ -861,10 +882,10 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
@@ -879,17 +900,137 @@
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
     </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="8"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="29">
+    <mergeCell ref="F12:F16"/>
+    <mergeCell ref="G12:G16"/>
+    <mergeCell ref="J12:J16"/>
+    <mergeCell ref="L12:L16"/>
+    <mergeCell ref="K2:K6"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="J2:J6"/>
+    <mergeCell ref="L2:L6"/>
     <mergeCell ref="F7:F11"/>
     <mergeCell ref="G7:G11"/>
     <mergeCell ref="A2:A6"/>
@@ -903,13 +1044,10 @@
     <mergeCell ref="C7:C11"/>
     <mergeCell ref="D7:D11"/>
     <mergeCell ref="E7:E11"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="G2:G6"/>
-    <mergeCell ref="J2:J6"/>
-    <mergeCell ref="L2:L6"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2:B6" r:id="rId1" display="'https://reqres.in/api/users?page=1" xr:uid="{AA02E096-2322-46F0-B127-13917E3254CA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>